<commit_message>
added local IP to authorized clients list
</commit_message>
<xml_diff>
--- a/GAMS_Computer Engineering_2015-2016.xlsx
+++ b/GAMS_Computer Engineering_2015-2016.xlsx
@@ -479,7 +479,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.625</c:v>
+                  <c:v>2.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -961,10 +961,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>2.625</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C4" s="2">
-        <v>1.111024302164449</v>
+        <v>1.105541596785133</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1940,37 +1940,37 @@
         <v>19</v>
       </c>
       <c r="J4" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K4" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L4" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M4" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N4" s="2">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="O4" s="2">
         <v>1</v>
       </c>
       <c r="P4" s="2">
-        <v>2.625</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="Q4" s="2">
-        <v>1.111024302164449</v>
+        <v>1.105541596785133</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
       </c>
       <c r="S4" s="2">
-        <v>2.625</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="T4" s="2">
-        <v>1.111024302164449</v>
+        <v>1.105541596785133</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2317,10 +2317,10 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1">
-        <v>2.625</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="T11" s="1">
-        <v>1.111024302164449</v>
+        <v>1.105541596785133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>